<commit_message>
close #101: Add check for 'desc_simples' column in dataframe
</commit_message>
<xml_diff>
--- a/input_data/data_errors_3/descricao.xlsx
+++ b/input_data/data_errors_3/descricao.xlsx
@@ -204,7 +204,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -234,13 +234,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -327,7 +320,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -434,13 +427,13 @@
   </sheetPr>
   <dimension ref="A1:Y866"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.42"/>

</xml_diff>